<commit_message>
modularized work process with an update, analyze, write work stream
</commit_message>
<xml_diff>
--- a/My_Finances.xlsx
+++ b/My_Finances.xlsx
@@ -2,14 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sep 2022" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Aug 2022" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="something" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -48,17 +47,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -137,10 +130,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -178,71 +171,69 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -266,53 +257,54 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
+                <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -322,7 +314,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -331,7 +323,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -340,7 +332,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -348,10 +340,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -380,7 +372,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -393,12 +385,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -418,7 +411,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:A1"/>
@@ -429,7 +422,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -507,10 +500,8 @@
           <t>Unkown</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Unkown</t>
-        </is>
+      <c r="H5" t="n">
+        <v>4235.66</v>
       </c>
     </row>
     <row r="6">
@@ -529,10 +520,8 @@
           <t>videogames</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>{videogames}</t>
-        </is>
+      <c r="D6" t="n">
+        <v>32.37</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -561,10 +550,8 @@
           <t>takeout</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>{takeout}</t>
-        </is>
+      <c r="D7" t="n">
+        <v>1172.51</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -615,10 +602,8 @@
           <t>Gym</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>{gym}</t>
-        </is>
+      <c r="B9" t="n">
+        <v>209.64</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -647,10 +632,8 @@
           <t>The Rounds</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>{the_rounds}</t>
-        </is>
+      <c r="B10" t="n">
+        <v>321.38</v>
       </c>
     </row>
     <row r="11">
@@ -659,10 +642,8 @@
           <t>Volo</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>{volo}</t>
-        </is>
+      <c r="B11" t="n">
+        <v>393.78</v>
       </c>
     </row>
     <row r="12">
@@ -680,179 +661,26 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Electric</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>{other_living_expenses}</t>
         </is>
       </c>
     </row>
-    <row r="14"/>
     <row r="15"/>
     <row r="16"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>main_template.xlsx</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>{timestamp}</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Total Liquid Assets</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>19490.03</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Living Expenses</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Groceries/Snacks</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>main_template.xlsx</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>{timestamp}</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>Total Liquid Assets</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>{total}</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="2" t="n"/>
-      <c r="B3" s="2" t="n"/>
-    </row>
-    <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Living Expenses</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Groceries/Snacks</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
-    </row>
-    <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="2" t="n"/>
-      <c r="B6" s="2" t="n"/>
-    </row>
-    <row r="7" ht="18.75" customHeight="1">
-      <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
-    </row>
-    <row r="8" ht="18.75" customHeight="1">
-      <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="n"/>
-    </row>
-    <row r="9" ht="18.75" customHeight="1">
-      <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
-    </row>
-    <row r="10" ht="18.75" customHeight="1">
-      <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
-    </row>
-    <row r="11" ht="18.75" customHeight="1">
-      <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
-    </row>
-    <row r="12" ht="18.75" customHeight="1">
-      <c r="A12" s="2" t="n"/>
-      <c r="B12" s="2" t="n"/>
-    </row>
-    <row r="13" ht="18.75" customHeight="1">
-      <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
-    </row>
-    <row r="14" ht="18.75" customHeight="1">
-      <c r="A14" s="2" t="n"/>
-      <c r="B14" s="2" t="n"/>
-    </row>
-    <row r="15" ht="18.75" customHeight="1">
-      <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>